<commit_message>
update working version 0.1
</commit_message>
<xml_diff>
--- a/results/Preliminaries-Australia.xlsx
+++ b/results/Preliminaries-Australia.xlsx
@@ -15,13 +15,14 @@
     <sheet name="Winning Coalitions" sheetId="6" r:id="rId6"/>
     <sheet name="Minimal Winning Coalitions" sheetId="7" r:id="rId7"/>
     <sheet name="Maximal Losing Coalitions" sheetId="8" r:id="rId8"/>
+    <sheet name="Unique Tying Coalitions" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5408" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5415" uniqueCount="670">
   <si>
     <t>Year</t>
   </si>
@@ -2025,6 +2026,12 @@
   </si>
   <si>
     <t xml:space="preserve">G -+KAP+LNP+Lab+Lib+Nat+X -+no </t>
+  </si>
+  <si>
+    <t>('CLP+Lib', 'Lab+Nat+no ')</t>
+  </si>
+  <si>
+    <t>('Lab+Nat+no ', 'CLP+Lib')</t>
   </si>
 </sst>
 </file>
@@ -32122,4 +32129,50 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>669</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>